<commit_message>
reverted to previous version
</commit_message>
<xml_diff>
--- a/app/utils/excel-parser-scripts/auction-daily-sample-to-become.xlsx
+++ b/app/utils/excel-parser-scripts/auction-daily-sample-to-become.xlsx
@@ -25,16 +25,16 @@
     <t xml:space="preserve">timestamp</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity HU&gt;RS </t>
+    <t xml:space="preserve">capacityHURS</t>
   </si>
   <si>
-    <t xml:space="preserve">Price HU&gt;RS </t>
+    <t xml:space="preserve">priceHURS</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity RS&gt;HU </t>
+    <t xml:space="preserve">capacityRSHU</t>
   </si>
   <si>
-    <t xml:space="preserve">Price RS&gt;HU </t>
+    <t xml:space="preserve">priceRSHU</t>
   </si>
 </sst>
 </file>
@@ -45,11 +45,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD\ HH:MM:SS"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -66,112 +67,16 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -179,23 +84,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,23 +109,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -247,91 +120,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -343,14 +139,14 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>

</xml_diff>

<commit_message>
finaly extracted headers only
</commit_message>
<xml_diff>
--- a/app/utils/excel-parser-scripts/auction-daily-sample-to-become.xlsx
+++ b/app/utils/excel-parser-scripts/auction-daily-sample-to-become.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">capacityHURS</t>
   </si>
   <si>
-    <t xml:space="preserve">priceHURS </t>
+    <t xml:space="preserve">priceHURS</t>
   </si>
   <si>
     <t xml:space="preserve">capacityRSHU</t>
@@ -139,7 +139,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
found a simple way to extract needed values
</commit_message>
<xml_diff>
--- a/app/utils/excel-parser-scripts/auction-daily-sample-to-become.xlsx
+++ b/app/utils/excel-parser-scripts/auction-daily-sample-to-become.xlsx
@@ -138,8 +138,8 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D1:E25 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>